<commit_message>
Correction of errors due to excel in French
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_BATS_Capacities_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_BATS_Capacities_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E39CF1-0FAD-41ED-BA04-2F2B3F4D3A42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{373ACBE0-DB1E-4AC3-A908-AA07BA98F3CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{82FCDFE4-D82B-4311-8D38-2D4266AAD1F5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECEBB67E-3135-438A-B60C-FAAFF21FBEA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,16 @@
     <t>Region</t>
   </si>
   <si>
-    <t>COM - Battery (Lead-acid) ELC Storage: DayNite (accompanying tech to represent power)</t>
-  </si>
-  <si>
-    <t>COM - Battery (Li-ion) ELC Storage: DayNite (accompanying tech to represent power)</t>
-  </si>
-  <si>
-    <t>RSD - Battery (Lead-acid) ELC Storage: DayNite (accompanying tech to represent power)</t>
-  </si>
-  <si>
-    <t>RSD - Battery (Li-ion) ELC Storage: DayNite (accompanying tech to represent power)</t>
+    <t>COM - Battery (Lead-acid) ELC Storage: DayNite</t>
+  </si>
+  <si>
+    <t>COM - Battery (Li-ion) ELC Storage: DayNite</t>
+  </si>
+  <si>
+    <t>RSD - Battery (Lead-acid) ELC Storage: DayNite</t>
+  </si>
+  <si>
+    <t>RSD - Battery (Li-ion) ELC Storage: DayNite</t>
   </si>
   <si>
     <t>BE</t>
@@ -139,6 +139,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -182,7 +185,7 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -511,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CB6E6E-7C5C-42AE-81B6-59426D2D24B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E7C5CD-DF7C-43BA-B246-BA4789E14A3B}">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -519,10 +522,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -555,10 +558,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>3.887</v>
+        <v>15.548999999999999</v>
       </c>
       <c r="D3" s="1">
-        <v>3.8849999999999998</v>
+        <v>15.541</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -566,10 +569,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>0.54500000000000004</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>0.54500000000000004</v>
+        <v>2.1779999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -577,13 +580,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>1.5740000000000001</v>
+        <v>6.2960000000000003</v>
       </c>
       <c r="C5" s="1">
         <v>0.17100000000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>1.575</v>
+        <v>6.3</v>
       </c>
       <c r="E5" s="1">
         <v>0.17100000000000001</v>
@@ -594,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>0.379</v>
       </c>
       <c r="D6" s="1">
-        <v>0.216</v>
+        <v>0.86499999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -605,10 +608,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>1.048</v>
+        <v>4.1920000000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>1.335</v>
+        <v>5.3419999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -616,10 +619,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>18.471</v>
+        <v>73.885999999999996</v>
       </c>
       <c r="D8" s="1">
-        <v>19.434000000000001</v>
+        <v>77.736999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -627,10 +630,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>3.0219999999999998</v>
+        <v>12.087999999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>3.0219999999999998</v>
+        <v>12.087999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,10 +641,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>0.47799999999999998</v>
+        <v>1.913</v>
       </c>
       <c r="D10" s="1">
-        <v>0.47799999999999998</v>
+        <v>1.913</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -649,10 +652,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>0.52400000000000002</v>
+        <v>2.097</v>
       </c>
       <c r="D11" s="1">
-        <v>1.1319999999999999</v>
+        <v>4.5279999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -660,10 +663,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>0.42699999999999999</v>
+        <v>1.7090000000000001</v>
       </c>
       <c r="D12" s="1">
-        <v>10.805999999999999</v>
+        <v>43.225000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -671,10 +674,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>3.4550000000000001</v>
+        <v>13.821999999999999</v>
       </c>
       <c r="D13" s="1">
-        <v>3.4580000000000002</v>
+        <v>13.834</v>
       </c>
       <c r="E13" s="1">
         <v>1.952</v>
@@ -685,7 +688,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="1">
-        <v>30.056000000000001</v>
+        <v>120.223</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -693,10 +696,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="1">
-        <v>0.22600000000000001</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="D15" s="1">
-        <v>0.24399999999999999</v>
+        <v>0.97399999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -704,10 +707,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>1.181</v>
+        <v>4.7220000000000004</v>
       </c>
       <c r="D16" s="1">
-        <v>1.1839999999999999</v>
+        <v>4.7359999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -715,13 +718,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>1.478</v>
+        <v>5.91</v>
       </c>
       <c r="C17" s="1">
         <v>0.93</v>
       </c>
       <c r="D17" s="1">
-        <v>1.478</v>
+        <v>5.91</v>
       </c>
       <c r="E17" s="1">
         <v>0.93</v>
@@ -732,10 +735,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>0.96199999999999997</v>
+        <v>3.847</v>
       </c>
       <c r="D18" s="1">
-        <v>0.97199999999999998</v>
+        <v>3.8860000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -743,10 +746,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>5.8380000000000001</v>
+        <v>23.350999999999999</v>
       </c>
       <c r="D19" s="1">
-        <v>5.8380000000000001</v>
+        <v>23.350999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -754,10 +757,10 @@
         <v>23</v>
       </c>
       <c r="B20" s="1">
-        <v>0.47299999999999998</v>
+        <v>1.89</v>
       </c>
       <c r="D20" s="1">
-        <v>0.47299999999999998</v>
+        <v>1.8919999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -765,10 +768,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="D21" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>0.16800000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -776,10 +779,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>9.6210000000000004</v>
+        <v>38.482999999999997</v>
       </c>
       <c r="D22" s="1">
-        <v>9.6210000000000004</v>
+        <v>38.482999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -787,10 +790,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="1">
-        <v>1.675</v>
+        <v>6.702</v>
       </c>
       <c r="D23" s="1">
-        <v>1.8240000000000001</v>
+        <v>7.298</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -798,10 +801,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="1">
-        <v>1.4339999999999999</v>
+        <v>5.734</v>
       </c>
       <c r="D24" s="1">
-        <v>2.605</v>
+        <v>10.417999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,10 +812,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="1">
-        <v>1.994</v>
+        <v>7.9749999999999996</v>
       </c>
       <c r="D25" s="1">
-        <v>3.7229999999999999</v>
+        <v>14.891999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -820,7 +823,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="1">
-        <v>1.2070000000000001</v>
+        <v>4.8280000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -828,13 +831,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="1">
-        <v>5.86</v>
+        <v>23.440999999999999</v>
       </c>
       <c r="C27" s="1">
         <v>6.7610000000000001</v>
       </c>
       <c r="D27" s="1">
-        <v>5.86</v>
+        <v>23.440999999999999</v>
       </c>
       <c r="E27" s="1">
         <v>6.7610000000000001</v>
@@ -845,10 +848,10 @@
         <v>31</v>
       </c>
       <c r="B28" s="1">
-        <v>0.55300000000000005</v>
+        <v>2.21</v>
       </c>
       <c r="D28" s="1">
-        <v>0.58399999999999996</v>
+        <v>2.3340000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,7 +859,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="1">
-        <v>0.216</v>
+        <v>0.86599999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -864,10 +867,10 @@
         <v>33</v>
       </c>
       <c r="B30" s="1">
-        <v>14.048999999999999</v>
+        <v>56.195</v>
       </c>
       <c r="D30" s="1">
-        <v>14.048999999999999</v>
+        <v>56.195</v>
       </c>
     </row>
   </sheetData>
@@ -875,5 +878,6 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct bats and H2 storage capacities
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_BATS_Capacities_2050.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_BATS_Capacities_2050.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{373ACBE0-DB1E-4AC3-A908-AA07BA98F3CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C143C914-FDB6-4244-BAE8-0E0616699DFB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECEBB67E-3135-438A-B60C-FAAFF21FBEA1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{35142C61-A1C5-45B7-AF59-033479965F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,22 +33,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>Process Description1</t>
+    <t>GW</t>
   </si>
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>COM - Battery (Lead-acid) ELC Storage: DayNite</t>
-  </si>
-  <si>
-    <t>COM - Battery (Li-ion) ELC Storage: DayNite</t>
-  </si>
-  <si>
-    <t>RSD - Battery (Lead-acid) ELC Storage: DayNite</t>
-  </si>
-  <si>
-    <t>RSD - Battery (Li-ion) ELC Storage: DayNite</t>
+    <t>COM - Battery (Lead-acid) ELC Storage: DayNite (accompanying tech to represent power)</t>
+  </si>
+  <si>
+    <t>COM - Battery (Li-ion) ELC Storage: DayNite (accompanying tech to represent power)</t>
+  </si>
+  <si>
+    <t>RSD - Battery (Lead-acid) ELC Storage: DayNite (accompanying tech to represent power)</t>
+  </si>
+  <si>
+    <t>RSD - Battery (Li-ion) ELC Storage: DayNite (accompanying tech to represent power)</t>
   </si>
   <si>
     <t>BE</t>
@@ -139,9 +139,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,20 +182,20 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
@@ -514,18 +511,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E7C5CD-DF7C-43BA-B246-BA4789E14A3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B8EBE9-91CF-4A0A-AA1D-C71BB3038E0D}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -537,19 +536,19 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -558,10 +557,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1">
-        <v>15.548999999999999</v>
+        <v>3.887</v>
       </c>
       <c r="D3" s="1">
-        <v>15.541</v>
+        <v>3.8849999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -569,10 +568,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>2.1779999999999999</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="D4" s="1">
-        <v>2.1779999999999999</v>
+        <v>0.54500000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -580,13 +579,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>6.2960000000000003</v>
+        <v>1.5740000000000001</v>
       </c>
       <c r="C5" s="1">
         <v>0.17100000000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>6.3</v>
+        <v>1.575</v>
       </c>
       <c r="E5" s="1">
         <v>0.17100000000000001</v>
@@ -597,10 +596,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="1">
-        <v>0.379</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>0.86499999999999999</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -608,10 +607,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="1">
-        <v>4.1920000000000002</v>
+        <v>1.048</v>
       </c>
       <c r="D7" s="1">
-        <v>5.3419999999999996</v>
+        <v>1.335</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -619,10 +618,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>73.885999999999996</v>
+        <v>18.471</v>
       </c>
       <c r="D8" s="1">
-        <v>77.736999999999995</v>
+        <v>19.434000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -630,10 +629,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>12.087999999999999</v>
+        <v>3.0219999999999998</v>
       </c>
       <c r="D9" s="1">
-        <v>12.087999999999999</v>
+        <v>3.0219999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,10 +640,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>1.913</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="D10" s="1">
-        <v>1.913</v>
+        <v>0.47799999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -652,10 +651,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>2.097</v>
+        <v>0.52400000000000002</v>
       </c>
       <c r="D11" s="1">
-        <v>4.5279999999999996</v>
+        <v>1.1319999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -663,10 +662,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>1.7090000000000001</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D12" s="1">
-        <v>43.225000000000001</v>
+        <v>10.805999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -674,10 +673,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>13.821999999999999</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="D13" s="1">
-        <v>13.834</v>
+        <v>3.4580000000000002</v>
       </c>
       <c r="E13" s="1">
         <v>1.952</v>
@@ -688,7 +687,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="1">
-        <v>120.223</v>
+        <v>30.056000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -696,10 +695,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="1">
-        <v>0.90200000000000002</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="D15" s="1">
-        <v>0.97399999999999998</v>
+        <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -707,10 +706,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>4.7220000000000004</v>
+        <v>1.181</v>
       </c>
       <c r="D16" s="1">
-        <v>4.7359999999999998</v>
+        <v>1.1839999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -718,13 +717,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>5.91</v>
+        <v>1.478</v>
       </c>
       <c r="C17" s="1">
         <v>0.93</v>
       </c>
       <c r="D17" s="1">
-        <v>5.91</v>
+        <v>1.478</v>
       </c>
       <c r="E17" s="1">
         <v>0.93</v>
@@ -735,10 +734,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="1">
-        <v>3.847</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="D18" s="1">
-        <v>3.8860000000000001</v>
+        <v>0.97199999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -746,10 +745,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="1">
-        <v>23.350999999999999</v>
+        <v>5.8380000000000001</v>
       </c>
       <c r="D19" s="1">
-        <v>23.350999999999999</v>
+        <v>5.8380000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -757,10 +756,10 @@
         <v>23</v>
       </c>
       <c r="B20" s="1">
-        <v>1.89</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="D20" s="1">
-        <v>1.8919999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -768,10 +767,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="1">
-        <v>0.16800000000000001</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D21" s="1">
-        <v>0.16800000000000001</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -779,10 +778,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="1">
-        <v>38.482999999999997</v>
+        <v>9.6210000000000004</v>
       </c>
       <c r="D22" s="1">
-        <v>38.482999999999997</v>
+        <v>9.6210000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -790,10 +789,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="1">
-        <v>6.702</v>
+        <v>1.675</v>
       </c>
       <c r="D23" s="1">
-        <v>7.298</v>
+        <v>1.8240000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -801,10 +800,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="1">
-        <v>5.734</v>
+        <v>1.4339999999999999</v>
       </c>
       <c r="D24" s="1">
-        <v>10.417999999999999</v>
+        <v>2.605</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -812,10 +811,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="1">
-        <v>7.9749999999999996</v>
+        <v>1.994</v>
       </c>
       <c r="D25" s="1">
-        <v>14.891999999999999</v>
+        <v>3.7229999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -823,7 +822,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="1">
-        <v>4.8280000000000003</v>
+        <v>1.2070000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -831,13 +830,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="1">
-        <v>23.440999999999999</v>
+        <v>5.86</v>
       </c>
       <c r="C27" s="1">
         <v>6.7610000000000001</v>
       </c>
       <c r="D27" s="1">
-        <v>23.440999999999999</v>
+        <v>5.86</v>
       </c>
       <c r="E27" s="1">
         <v>6.7610000000000001</v>
@@ -848,10 +847,10 @@
         <v>31</v>
       </c>
       <c r="B28" s="1">
-        <v>2.21</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="D28" s="1">
-        <v>2.3340000000000001</v>
+        <v>0.58399999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -859,7 +858,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="1">
-        <v>0.86599999999999999</v>
+        <v>0.216</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -867,10 +866,10 @@
         <v>33</v>
       </c>
       <c r="B30" s="1">
-        <v>56.195</v>
+        <v>14.048999999999999</v>
       </c>
       <c r="D30" s="1">
-        <v>56.195</v>
+        <v>14.048999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>